<commit_message>
Fixed missing location data for HOU-SBFC (Week 3)
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-hou-sbfc-042916.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-hou-sbfc-042916.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/wosostats/source/excel/nwsl-2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12020" yWindow="620" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="1480" windowWidth="22740" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">match!$A$1:$T$1611</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17280" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17282" uniqueCount="241">
   <si>
     <t>event</t>
   </si>
@@ -748,6 +747,12 @@
   </si>
   <si>
     <t>HAYES</t>
+  </si>
+  <si>
+    <t>AMR</t>
+  </si>
+  <si>
+    <t>DR</t>
   </si>
 </sst>
 </file>
@@ -1687,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A980" zoomScale="92" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G1005" sqref="G1005"/>
+    <sheetView tabSelected="1" topLeftCell="A1565" zoomScale="92" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="N1580" sqref="N1580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23916,7 +23921,9 @@
       <c r="M536" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="N536" s="12"/>
+      <c r="N536" s="12" t="s">
+        <v>239</v>
+      </c>
       <c r="O536" s="12"/>
       <c r="P536" s="12"/>
       <c r="Q536" s="12"/>
@@ -27992,7 +27999,9 @@
       <c r="M635" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="N635" s="12"/>
+      <c r="N635" s="12" t="s">
+        <v>240</v>
+      </c>
       <c r="O635" s="12"/>
       <c r="P635" s="12"/>
       <c r="Q635" s="12"/>
@@ -42871,7 +42880,7 @@
         <v>123</v>
       </c>
       <c r="N940" s="38" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="O940" s="38" t="s">
         <v>169</v>
@@ -48086,7 +48095,7 @@
         <v>123</v>
       </c>
       <c r="N1026" s="38" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="O1026" s="38" t="s">
         <v>169</v>
@@ -49367,7 +49376,7 @@
         <v>123</v>
       </c>
       <c r="N1047" s="38" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="O1047" s="38" t="s">
         <v>169</v>
@@ -53090,7 +53099,7 @@
         <v>189</v>
       </c>
       <c r="N1108" s="38" t="s">
-        <v>169</v>
+        <v>116</v>
       </c>
       <c r="O1108" s="38" t="s">
         <v>169</v>
@@ -62218,7 +62227,7 @@
         <v>123</v>
       </c>
       <c r="N1258" s="38" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="O1258" s="38" t="s">
         <v>169</v>
@@ -78837,7 +78846,7 @@
         <v>123</v>
       </c>
       <c r="N1533" s="38" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="O1533" s="38" t="s">
         <v>169</v>
@@ -81641,7 +81650,7 @@
         <v>123</v>
       </c>
       <c r="N1579" s="38" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="O1579" s="38" t="s">
         <v>169</v>

</xml_diff>

<commit_message>
Changed formatting on several Excel source files
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-hou-sbfc-042916.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-hou-sbfc-042916.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/wosostats/source/excel/nwsl-2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17283" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17339" uniqueCount="241">
   <si>
     <t>event</t>
   </si>
@@ -1133,287 +1133,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <color theme="1"/>
@@ -1970,7 +1690,7 @@
   <dimension ref="A1:Z1611"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2068,8 +1788,12 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="C2" s="20" t="s">
         <v>20</v>
       </c>
@@ -2132,8 +1856,12 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C3" s="20" t="s">
         <v>31</v>
       </c>
@@ -2196,8 +1924,12 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C4" s="20" t="s">
         <v>31</v>
       </c>
@@ -2260,8 +1992,12 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C5" s="20" t="s">
         <v>31</v>
       </c>
@@ -2324,8 +2060,12 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C6" s="20" t="s">
         <v>31</v>
       </c>
@@ -2386,8 +2126,12 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C7" s="23" t="s">
         <v>67</v>
       </c>
@@ -2446,8 +2190,12 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C8" s="23" t="s">
         <v>67</v>
       </c>
@@ -2502,8 +2250,12 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C9" s="23" t="s">
         <v>67</v>
       </c>
@@ -2558,8 +2310,12 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C10" s="23" t="s">
         <v>87</v>
       </c>
@@ -2614,8 +2370,12 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C11" s="20" t="s">
         <v>87</v>
       </c>
@@ -2670,8 +2430,12 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C12" s="20" t="s">
         <v>87</v>
       </c>
@@ -2724,8 +2488,12 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C13" s="20" t="s">
         <v>87</v>
       </c>
@@ -2778,8 +2546,12 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C14" s="20" t="s">
         <v>87</v>
       </c>
@@ -2832,8 +2604,12 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21" t="s">
         <v>21</v>
@@ -2880,8 +2656,12 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C16" s="20" t="s">
         <v>20</v>
       </c>
@@ -2932,8 +2712,12 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C17" s="20" t="s">
         <v>31</v>
       </c>
@@ -2982,8 +2766,12 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C18" s="20" t="s">
         <v>31</v>
       </c>
@@ -3026,8 +2814,12 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C19" s="20" t="s">
         <v>31</v>
       </c>
@@ -3070,8 +2862,12 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C20" s="23" t="s">
         <v>31</v>
       </c>
@@ -3114,8 +2910,12 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C21" s="23" t="s">
         <v>67</v>
       </c>
@@ -3158,8 +2958,12 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C22" s="23" t="s">
         <v>67</v>
       </c>
@@ -3202,8 +3006,12 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C23" s="23" t="s">
         <v>67</v>
       </c>
@@ -3246,8 +3054,12 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C24" s="20" t="s">
         <v>67</v>
       </c>
@@ -3290,8 +3102,12 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C25" s="20" t="s">
         <v>87</v>
       </c>
@@ -3332,8 +3148,12 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C26" s="28" t="s">
         <v>87</v>
       </c>
@@ -3374,8 +3194,12 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C27" s="30" t="s">
         <v>67</v>
       </c>
@@ -3416,8 +3240,12 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="D28" s="25" t="s">
         <v>122</v>
@@ -3454,8 +3282,12 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="C29" s="8"/>
       <c r="D29" s="25" t="s">
         <v>122</v>
@@ -81917,7 +81749,7 @@
     </row>
     <row r="1567" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1567" s="8">
-        <f t="shared" ref="A1567:A1611" si="24">IF(OR(F1567="",F1567="-",F1567=" "),A1566,A1566+1)</f>
+        <f t="shared" ref="A1567:A1610" si="24">IF(OR(F1567="",F1567="-",F1567=" "),A1566,A1566+1)</f>
         <v>1427</v>
       </c>
       <c r="B1567" s="23" t="s">
@@ -84668,88 +84500,88 @@
   <autoFilter ref="A1:T1611"/>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576 L1:L1048576">
-    <cfRule type="containsText" dxfId="55" priority="1" operator="containsText" text="stanton">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="stanton">
       <formula>NOT(ISERROR(SEARCH("stanton",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="schulmann">
+    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="schulmann">
       <formula>NOT(ISERROR(SEARCH("schulmann",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="conheeney">
+    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="conheeney">
       <formula>NOT(ISERROR(SEARCH("conheeney",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="4" operator="containsText" text="kai">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="kai">
       <formula>NOT(ISERROR(SEARCH("kai",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="5" operator="containsText" text="rodriguez">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="rodriguez">
       <formula>NOT(ISERROR(SEARCH("rodriguez",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="6" operator="containsText" text="hayes">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="hayes">
       <formula>NOT(ISERROR(SEARCH("hayes",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="killion">
+    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="killion">
       <formula>NOT(ISERROR(SEARCH("killion",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="8" operator="containsText" text="nick">
+    <cfRule type="containsText" dxfId="20" priority="8" operator="containsText" text="nick">
       <formula>NOT(ISERROR(SEARCH("nick",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="lytle">
+    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="lytle">
       <formula>NOT(ISERROR(SEARCH("lytle",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="simon">
+    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="simon">
       <formula>NOT(ISERROR(SEARCH("simon",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="rampone">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="rampone">
       <formula>NOT(ISERROR(SEARCH("rampone",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="12" operator="containsText" text="Skroski">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Skroski">
       <formula>NOT(ISERROR(SEARCH("Skroski",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="13" operator="containsText" text="O'hara">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="O'hara">
       <formula>NOT(ISERROR(SEARCH("O'hara",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="14" operator="containsText" text="Stanley">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Stanley">
       <formula>NOT(ISERROR(SEARCH("Stanley",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="15" operator="containsText" text="Ochs">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Ochs">
       <formula>NOT(ISERROR(SEARCH("Ochs",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="16" operator="containsText" text="Beckie">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Beckie">
       <formula>NOT(ISERROR(SEARCH("Beckie",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="O'Sullivan">
+    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="O'Sullivan">
       <formula>NOT(ISERROR(SEARCH("O'Sullivan",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Ubogagu">
+    <cfRule type="containsText" dxfId="10" priority="18" operator="containsText" text="Ubogagu">
       <formula>NOT(ISERROR(SEARCH("Ubogagu",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="19" operator="containsText" text="Ohai">
+    <cfRule type="containsText" dxfId="9" priority="19" operator="containsText" text="Ohai">
       <formula>NOT(ISERROR(SEARCH("Ohai",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="20" operator="containsText" text="Daly">
+    <cfRule type="containsText" dxfId="8" priority="20" operator="containsText" text="Daly">
       <formula>NOT(ISERROR(SEARCH("Daly",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="21" operator="containsText" text="heap">
+    <cfRule type="containsText" dxfId="7" priority="21" operator="containsText" text="heap">
       <formula>NOT(ISERROR(SEARCH("heap",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="22" operator="containsText" text="andressa">
+    <cfRule type="containsText" dxfId="6" priority="22" operator="containsText" text="andressa">
       <formula>NOT(ISERROR(SEARCH("andressa",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="23" operator="containsText" text="privett">
+    <cfRule type="containsText" dxfId="5" priority="23" operator="containsText" text="privett">
       <formula>NOT(ISERROR(SEARCH("privett",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="24" operator="containsText" text="poliana">
+    <cfRule type="containsText" dxfId="4" priority="24" operator="containsText" text="poliana">
       <formula>NOT(ISERROR(SEARCH("poliana",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="brush">
+    <cfRule type="containsText" dxfId="3" priority="25" operator="containsText" text="brush">
       <formula>NOT(ISERROR(SEARCH("brush",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="moros">
+    <cfRule type="containsText" dxfId="2" priority="26" operator="containsText" text="moros">
       <formula>NOT(ISERROR(SEARCH("moros",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="chapman">
+    <cfRule type="containsText" dxfId="1" priority="27" operator="containsText" text="chapman">
       <formula>NOT(ISERROR(SEARCH("chapman",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="williams">
+    <cfRule type="containsText" dxfId="0" priority="28" operator="containsText" text="williams">
       <formula>NOT(ISERROR(SEARCH("williams",E1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>